<commit_message>
Nieuwe conclusie voor nieuwe project
</commit_message>
<xml_diff>
--- a/Documentatie/Logboek.xlsx
+++ b/Documentatie/Logboek.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Menno\Downloads\school\project\raspberry\project-5\Documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project 5\project-5\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="12192"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Wat?</t>
   </si>
@@ -132,12 +132,21 @@
   </si>
   <si>
     <t>Gelukt!</t>
+  </si>
+  <si>
+    <t>12:40 - 12:50</t>
+  </si>
+  <si>
+    <t>Overleggen over voortgang van project met Roode</t>
+  </si>
+  <si>
+    <t>We zijn op de conclusie gekomen dat  het lastig is om verder te blijven werken aan dit project. Door deze reden hebben we besloten om verder te gaan werken aan het adres boekje.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -170,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -180,6 +189,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -222,15 +234,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel4" displayName="Tabel4" ref="A1:F70" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel4" displayName="Tabel4" ref="A1:F70" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F70"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Datum" dataDxfId="6"/>
-    <tableColumn id="2" name="Tijd" dataDxfId="5"/>
-    <tableColumn id="3" name="Wat?" dataDxfId="4"/>
-    <tableColumn id="5" name="Wie?" dataDxfId="3"/>
-    <tableColumn id="7" name="opmerkingen?" dataDxfId="2"/>
-    <tableColumn id="9" name="gaat hierna werken aan?" dataDxfId="1"/>
+    <tableColumn id="1" name="Datum" dataDxfId="5"/>
+    <tableColumn id="2" name="Tijd" dataDxfId="4"/>
+    <tableColumn id="3" name="Wat?" dataDxfId="3"/>
+    <tableColumn id="5" name="Wie?" dataDxfId="2"/>
+    <tableColumn id="7" name="opmerkingen?" dataDxfId="1"/>
+    <tableColumn id="9" name="gaat hierna werken aan?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -535,17 +547,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -568,7 +580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>42776</v>
       </c>
@@ -587,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42776</v>
       </c>
@@ -606,7 +618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>42776</v>
       </c>
@@ -629,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>42776</v>
       </c>
@@ -650,7 +662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>42776</v>
       </c>
@@ -671,7 +683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>42776</v>
       </c>
@@ -687,7 +699,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>42776</v>
       </c>
@@ -705,7 +717,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>42776</v>
       </c>
@@ -723,7 +735,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>42776</v>
       </c>
@@ -741,15 +753,25 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>42811</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -757,7 +779,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -765,7 +787,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -773,7 +795,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -781,7 +803,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -789,7 +811,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -797,7 +819,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -805,7 +827,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -813,7 +835,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -821,7 +843,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -829,7 +851,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -837,7 +859,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -845,7 +867,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -853,7 +875,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -861,7 +883,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -869,7 +891,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -877,7 +899,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -885,7 +907,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -893,7 +915,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -901,7 +923,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -909,7 +931,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -917,7 +939,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -925,7 +947,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -933,7 +955,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -941,7 +963,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -949,7 +971,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -957,7 +979,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -965,7 +987,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -973,7 +995,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -981,7 +1003,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -989,7 +1011,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -997,7 +1019,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1005,7 +1027,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1013,7 +1035,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1021,7 +1043,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1029,7 +1051,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1037,7 +1059,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1045,7 +1067,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1053,7 +1075,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1061,7 +1083,7 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1069,7 +1091,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1077,7 +1099,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1085,7 +1107,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1093,7 +1115,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1101,7 +1123,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1109,7 +1131,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1117,7 +1139,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1125,7 +1147,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -1133,7 +1155,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -1141,7 +1163,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -1149,7 +1171,7 @@
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -1157,7 +1179,7 @@
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
@@ -1165,7 +1187,7 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -1173,7 +1195,7 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -1181,7 +1203,7 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1189,7 +1211,7 @@
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -1197,7 +1219,7 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -1205,7 +1227,7 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -1213,7 +1235,7 @@
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>

</xml_diff>